<commit_message>
variable initialization for VS RSVP test cases
</commit_message>
<xml_diff>
--- a/NewArrivals/virtualShowData.xlsx
+++ b/NewArrivals/virtualShowData.xlsx
@@ -443,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,21 +457,20 @@
     <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="22" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -494,37 +493,37 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="P1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
+      <c r="Q1" t="s">
         <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -546,38 +545,38 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="H2">
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+      <c r="P2">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="Q2">
         <v>2019</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>